<commit_message>
Fixed Risk Assessment Calculator
</commit_message>
<xml_diff>
--- a/OWASPv4_Checklist.xlsx
+++ b/OWASPv4_Checklist.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26101"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prathan/Github/OWASP-Testing-Checklist/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\OWASP-Testing-Checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="22740" windowHeight="12740"/>
+    <workbookView xWindow="120" yWindow="465" windowWidth="22740" windowHeight="12735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Testing Checklist" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,6 @@
     <sheet name="Risk Assessment Calculator" sheetId="2" r:id="rId3"/>
     <sheet name="References" sheetId="3" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Awareness">References!$M$3:$M$7</definedName>
     <definedName name="EaseofExploit">References!$K$3:$K$7</definedName>
@@ -39,7 +36,7 @@
     <definedName name="result">'Testing Checklist'!$A$128:$A$130</definedName>
     <definedName name="SkillRequired">References!$A$3:$A$8</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -55,7 +52,7 @@
     <author>pphongthiproek</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0">
+    <comment ref="A5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="1">
+    <comment ref="F5" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0">
+    <comment ref="A6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="1">
+    <comment ref="F6" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="1">
+    <comment ref="A7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="1">
+    <comment ref="F7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -139,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="1">
+    <comment ref="A8" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -153,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="1">
+    <comment ref="F8" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="1">
+    <comment ref="A11" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -181,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="1">
+    <comment ref="F11" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -195,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="1">
+    <comment ref="A12" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -209,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="1">
+    <comment ref="F12" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="1">
+    <comment ref="A13" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -237,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="1">
+    <comment ref="F13" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -251,7 +248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="1">
+    <comment ref="A14" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -265,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="1">
+    <comment ref="F14" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2167,18 +2164,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2204,6 +2189,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3629,19 +3626,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4098,39 +4082,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A76" workbookViewId="0">
       <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="53.6640625" style="40" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" style="40" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
         <v>333</v>
       </c>
       <c r="B1" s="49"/>
       <c r="E1" s="29"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
         <v>122</v>
       </c>
       <c r="B2" s="50"/>
     </row>
-    <row r="3" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="36"/>
       <c r="B3" s="36"/>
       <c r="C3" s="40"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" s="20" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>0</v>
       </c>
@@ -4150,7 +4134,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>126</v>
       </c>
@@ -4167,7 +4151,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>127</v>
       </c>
@@ -4184,7 +4168,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>128</v>
       </c>
@@ -4201,7 +4185,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>129</v>
       </c>
@@ -4218,7 +4202,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>130</v>
       </c>
@@ -4235,7 +4219,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>131</v>
       </c>
@@ -4252,7 +4236,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>132</v>
       </c>
@@ -4269,7 +4253,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="20" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" s="20" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>133</v>
       </c>
@@ -4287,7 +4271,7 @@
       </c>
       <c r="F12" s="29"/>
     </row>
-    <row r="13" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>134</v>
       </c>
@@ -4305,7 +4289,7 @@
       </c>
       <c r="F13" s="29"/>
     </row>
-    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>135</v>
       </c>
@@ -4323,14 +4307,14 @@
       </c>
       <c r="F14" s="29"/>
     </row>
-    <row r="15" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
       <c r="B15" s="7"/>
       <c r="C15" s="41"/>
       <c r="D15" s="44"/>
       <c r="E15" s="21"/>
     </row>
-    <row r="16" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
         <v>125</v>
       </c>
@@ -4350,7 +4334,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>145</v>
       </c>
@@ -4367,7 +4351,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>146</v>
       </c>
@@ -4384,7 +4368,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
         <v>147</v>
       </c>
@@ -4401,7 +4385,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>148</v>
       </c>
@@ -4418,7 +4402,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
         <v>149</v>
       </c>
@@ -4435,7 +4419,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>150</v>
       </c>
@@ -4452,7 +4436,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="20" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" s="20" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>151</v>
       </c>
@@ -4470,7 +4454,7 @@
       </c>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>152</v>
       </c>
@@ -4487,14 +4471,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="7"/>
       <c r="C25" s="41"/>
       <c r="D25" s="44"/>
       <c r="E25" s="21"/>
     </row>
-    <row r="26" spans="1:6" s="29" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" s="29" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
         <v>161</v>
       </c>
@@ -4514,7 +4498,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="29" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" s="29" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>162</v>
       </c>
@@ -4531,7 +4515,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
         <v>163</v>
       </c>
@@ -4549,7 +4533,7 @@
       </c>
       <c r="F28" s="29"/>
     </row>
-    <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>164</v>
       </c>
@@ -4567,7 +4551,7 @@
       </c>
       <c r="F29" s="29"/>
     </row>
-    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
         <v>165</v>
       </c>
@@ -4585,7 +4569,7 @@
       </c>
       <c r="F30" s="29"/>
     </row>
-    <row r="31" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
         <v>166</v>
       </c>
@@ -4603,7 +4587,7 @@
       </c>
       <c r="F31" s="29"/>
     </row>
-    <row r="32" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
         <v>167</v>
       </c>
@@ -4621,7 +4605,7 @@
       </c>
       <c r="F32" s="29"/>
     </row>
-    <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
         <v>168</v>
       </c>
@@ -4639,14 +4623,14 @@
       </c>
       <c r="F33" s="29"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="20"/>
       <c r="C34" s="41"/>
       <c r="D34" s="44"/>
       <c r="E34" s="21"/>
       <c r="F34" s="29"/>
     </row>
-    <row r="35" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" s="20" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="26" t="s">
         <v>1</v>
       </c>
@@ -4666,7 +4650,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
         <v>176</v>
       </c>
@@ -4683,7 +4667,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
         <v>177</v>
       </c>
@@ -4700,7 +4684,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
         <v>178</v>
       </c>
@@ -4717,7 +4701,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
         <v>179</v>
       </c>
@@ -4734,7 +4718,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
         <v>180</v>
       </c>
@@ -4751,7 +4735,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
         <v>181</v>
       </c>
@@ -4768,7 +4752,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="20" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" s="20" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
         <v>182</v>
       </c>
@@ -4786,7 +4770,7 @@
       </c>
       <c r="F42"/>
     </row>
-    <row r="43" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
         <v>183</v>
       </c>
@@ -4803,7 +4787,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
         <v>184</v>
       </c>
@@ -4820,7 +4804,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
         <v>185</v>
       </c>
@@ -4837,14 +4821,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20"/>
       <c r="B46" s="7"/>
       <c r="C46" s="41"/>
       <c r="D46" s="44"/>
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="26" t="s">
         <v>2</v>
       </c>
@@ -4864,7 +4848,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="20" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6" s="20" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
         <v>196</v>
       </c>
@@ -4881,7 +4865,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
         <v>197</v>
       </c>
@@ -4898,7 +4882,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
         <v>198</v>
       </c>
@@ -4915,7 +4899,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="20" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
         <v>199</v>
       </c>
@@ -4933,7 +4917,7 @@
       </c>
       <c r="F51"/>
     </row>
-    <row r="52" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="40"/>
@@ -4941,7 +4925,7 @@
       <c r="E52" s="29"/>
       <c r="F52" s="29"/>
     </row>
-    <row r="53" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="26" t="s">
         <v>204</v>
       </c>
@@ -4961,7 +4945,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
         <v>205</v>
       </c>
@@ -4978,7 +4962,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
         <v>206</v>
       </c>
@@ -4995,7 +4979,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
         <v>207</v>
       </c>
@@ -5013,7 +4997,7 @@
       </c>
       <c r="F56" s="20"/>
     </row>
-    <row r="57" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
         <v>208</v>
       </c>
@@ -5030,7 +5014,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
         <v>209</v>
       </c>
@@ -5047,7 +5031,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
         <v>210</v>
       </c>
@@ -5064,7 +5048,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
         <v>211</v>
       </c>
@@ -5081,7 +5065,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
         <v>212</v>
       </c>
@@ -5099,7 +5083,7 @@
       </c>
       <c r="F61" s="20"/>
     </row>
-    <row r="62" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="20"/>
       <c r="B62" s="7"/>
       <c r="C62" s="42"/>
@@ -5107,7 +5091,7 @@
       <c r="E62" s="23"/>
       <c r="F62" s="20"/>
     </row>
-    <row r="63" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:6" s="29" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" s="28" t="s">
         <v>3</v>
       </c>
@@ -5127,7 +5111,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
         <v>248</v>
       </c>
@@ -5144,7 +5128,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
         <v>249</v>
       </c>
@@ -5161,7 +5145,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
         <v>250</v>
       </c>
@@ -5179,7 +5163,7 @@
       </c>
       <c r="F66" s="20"/>
     </row>
-    <row r="67" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
         <v>251</v>
       </c>
@@ -5196,7 +5180,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A68" s="37" t="s">
         <v>252</v>
       </c>
@@ -5213,7 +5197,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A69" s="20"/>
       <c r="B69" s="7" t="s">
         <v>226</v>
@@ -5228,7 +5212,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A70" s="20"/>
       <c r="B70" s="7" t="s">
         <v>227</v>
@@ -5243,7 +5227,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A71" s="20"/>
       <c r="B71" s="7" t="s">
         <v>228</v>
@@ -5258,7 +5242,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="20" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:6" s="20" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="B72" s="7" t="s">
         <v>229</v>
       </c>
@@ -5273,7 +5257,7 @@
       </c>
       <c r="F72"/>
     </row>
-    <row r="73" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A73" s="20"/>
       <c r="B73" s="7" t="s">
         <v>230</v>
@@ -5288,7 +5272,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A74" s="20"/>
       <c r="B74" s="7" t="s">
         <v>231</v>
@@ -5303,7 +5287,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
         <v>253</v>
       </c>
@@ -5320,7 +5304,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
         <v>254</v>
       </c>
@@ -5337,7 +5321,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A77" s="20" t="s">
         <v>255</v>
       </c>
@@ -5354,7 +5338,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="20" t="s">
         <v>256</v>
       </c>
@@ -5371,7 +5355,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="20" t="s">
         <v>257</v>
       </c>
@@ -5388,7 +5372,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A80" s="20" t="s">
         <v>258</v>
       </c>
@@ -5405,7 +5389,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="20" t="s">
         <v>259</v>
       </c>
@@ -5423,7 +5407,7 @@
       </c>
       <c r="F81" s="29"/>
     </row>
-    <row r="82" spans="1:6" s="20" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:6" s="20" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="B82" s="7" t="s">
         <v>239</v>
       </c>
@@ -5438,7 +5422,7 @@
       </c>
       <c r="F82" s="29"/>
     </row>
-    <row r="83" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A83" s="20"/>
       <c r="B83" s="7" t="s">
         <v>240</v>
@@ -5454,7 +5438,7 @@
       </c>
       <c r="F83" s="29"/>
     </row>
-    <row r="84" spans="1:6" ht="52" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A84" s="20" t="s">
         <v>260</v>
       </c>
@@ -5472,7 +5456,7 @@
       </c>
       <c r="F84" s="29"/>
     </row>
-    <row r="85" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A85" s="20" t="s">
         <v>261</v>
       </c>
@@ -5490,7 +5474,7 @@
       </c>
       <c r="F85" s="29"/>
     </row>
-    <row r="86" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="20"/>
       <c r="B86" s="7" t="s">
         <v>243</v>
@@ -5502,7 +5486,7 @@
       </c>
       <c r="F86" s="29"/>
     </row>
-    <row r="87" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="20"/>
       <c r="B87" s="7" t="s">
         <v>244</v>
@@ -5514,7 +5498,7 @@
       </c>
       <c r="F87" s="29"/>
     </row>
-    <row r="88" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="20"/>
       <c r="B88" s="7" t="s">
         <v>245</v>
@@ -5526,7 +5510,7 @@
       </c>
       <c r="F88" s="29"/>
     </row>
-    <row r="89" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A89" s="20" t="s">
         <v>262</v>
       </c>
@@ -5544,7 +5528,7 @@
       </c>
       <c r="F89" s="29"/>
     </row>
-    <row r="90" spans="1:6" ht="65" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A90" s="20" t="s">
         <v>263</v>
       </c>
@@ -5562,14 +5546,14 @@
       </c>
       <c r="F90" s="29"/>
     </row>
-    <row r="91" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="20"/>
       <c r="B91" s="7"/>
       <c r="C91" s="43"/>
       <c r="D91" s="45"/>
       <c r="E91" s="23"/>
     </row>
-    <row r="92" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="26" t="s">
         <v>264</v>
       </c>
@@ -5589,7 +5573,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="20" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:6" s="20" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A93" s="20" t="s">
         <v>267</v>
       </c>
@@ -5607,7 +5591,7 @@
       </c>
       <c r="F93" s="29"/>
     </row>
-    <row r="94" spans="1:6" s="20" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:6" s="20" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="20" t="s">
         <v>268</v>
       </c>
@@ -5625,14 +5609,14 @@
       </c>
       <c r="F94" s="29"/>
     </row>
-    <row r="95" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B95" s="7"/>
       <c r="C95" s="41"/>
       <c r="D95" s="44"/>
       <c r="E95" s="21"/>
       <c r="F95" s="29"/>
     </row>
-    <row r="96" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="26" t="s">
         <v>269</v>
       </c>
@@ -5652,7 +5636,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" s="20" t="s">
         <v>273</v>
       </c>
@@ -5670,7 +5654,7 @@
       </c>
       <c r="F97" s="29"/>
     </row>
-    <row r="98" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="20" t="s">
         <v>274</v>
       </c>
@@ -5688,7 +5672,7 @@
       </c>
       <c r="F98" s="29"/>
     </row>
-    <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:6" ht="84" x14ac:dyDescent="0.2">
       <c r="A99" s="20" t="s">
         <v>275</v>
       </c>
@@ -5706,13 +5690,13 @@
       </c>
       <c r="F99" s="29"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C100" s="43"/>
       <c r="D100" s="45"/>
       <c r="E100" s="23"/>
       <c r="F100" s="29"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" s="26" t="s">
         <v>276</v>
       </c>
@@ -5732,7 +5716,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A102" s="20" t="s">
         <v>277</v>
       </c>
@@ -5749,7 +5733,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="20" t="s">
         <v>278</v>
       </c>
@@ -5766,7 +5750,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="108" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A104" s="20" t="s">
         <v>279</v>
       </c>
@@ -5784,7 +5768,7 @@
       </c>
       <c r="F104" s="20"/>
     </row>
-    <row r="105" spans="1:6" ht="84" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:6" ht="84" x14ac:dyDescent="0.2">
       <c r="A105" s="20" t="s">
         <v>280</v>
       </c>
@@ -5802,7 +5786,7 @@
       </c>
       <c r="F105" s="20"/>
     </row>
-    <row r="106" spans="1:6" ht="84" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:6" ht="84" x14ac:dyDescent="0.2">
       <c r="A106" s="20" t="s">
         <v>281</v>
       </c>
@@ -5820,7 +5804,7 @@
       </c>
       <c r="F106" s="20"/>
     </row>
-    <row r="107" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:6" ht="72" x14ac:dyDescent="0.2">
       <c r="A107" s="20" t="s">
         <v>282</v>
       </c>
@@ -5838,7 +5822,7 @@
       </c>
       <c r="F107" s="20"/>
     </row>
-    <row r="108" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A108" s="20" t="s">
         <v>283</v>
       </c>
@@ -5856,7 +5840,7 @@
       </c>
       <c r="F108" s="20"/>
     </row>
-    <row r="109" spans="1:6" ht="72" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A109" s="20" t="s">
         <v>284</v>
       </c>
@@ -5874,7 +5858,7 @@
       </c>
       <c r="F109" s="20"/>
     </row>
-    <row r="110" spans="1:6" ht="60" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A110" s="20" t="s">
         <v>285</v>
       </c>
@@ -5892,7 +5876,7 @@
       </c>
       <c r="F110" s="20"/>
     </row>
-    <row r="111" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="20"/>
       <c r="B111" s="7"/>
       <c r="C111" s="41"/>
@@ -5900,7 +5884,7 @@
       <c r="E111" s="21"/>
       <c r="F111" s="20"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="26" t="s">
         <v>295</v>
       </c>
@@ -5920,7 +5904,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="20" t="s">
         <v>296</v>
       </c>
@@ -5938,7 +5922,7 @@
       </c>
       <c r="F113" s="29"/>
     </row>
-    <row r="114" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A114" s="20" t="s">
         <v>297</v>
       </c>
@@ -5956,7 +5940,7 @@
       </c>
       <c r="F114" s="29"/>
     </row>
-    <row r="115" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A115" s="20" t="s">
         <v>298</v>
       </c>
@@ -5974,7 +5958,7 @@
       </c>
       <c r="F115" s="20"/>
     </row>
-    <row r="116" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A116" s="20" t="s">
         <v>299</v>
       </c>
@@ -5992,7 +5976,7 @@
       </c>
       <c r="F116" s="20"/>
     </row>
-    <row r="117" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A117" s="20" t="s">
         <v>300</v>
       </c>
@@ -6010,7 +5994,7 @@
       </c>
       <c r="F117" s="20"/>
     </row>
-    <row r="118" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="20" t="s">
         <v>301</v>
       </c>
@@ -6028,7 +6012,7 @@
       </c>
       <c r="F118" s="20"/>
     </row>
-    <row r="119" spans="1:6" ht="24" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A119" s="20" t="s">
         <v>302</v>
       </c>
@@ -6046,7 +6030,7 @@
       </c>
       <c r="F119" s="20"/>
     </row>
-    <row r="120" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A120" s="20" t="s">
         <v>303</v>
       </c>
@@ -6064,7 +6048,7 @@
       </c>
       <c r="F120" s="20"/>
     </row>
-    <row r="121" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="20" t="s">
         <v>304</v>
       </c>
@@ -6082,7 +6066,7 @@
       </c>
       <c r="F121" s="20"/>
     </row>
-    <row r="122" spans="1:6" ht="48" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A122" s="20" t="s">
         <v>305</v>
       </c>
@@ -6099,7 +6083,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A123" s="20" t="s">
         <v>306</v>
       </c>
@@ -6117,7 +6101,7 @@
       </c>
       <c r="F123" s="29"/>
     </row>
-    <row r="124" spans="1:6" ht="36" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A124" s="20" t="s">
         <v>307</v>
       </c>
@@ -6135,36 +6119,36 @@
       </c>
       <c r="F124" s="29"/>
     </row>
-    <row r="125" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="20"/>
       <c r="B125" s="7"/>
       <c r="C125" s="41"/>
       <c r="D125" s="44"/>
       <c r="E125" s="21"/>
     </row>
-    <row r="126" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="37"/>
       <c r="B126" s="7"/>
       <c r="C126" s="41"/>
       <c r="D126" s="44"/>
       <c r="E126" s="21"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="25" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="25" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="25" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="25" t="s">
         <v>7</v>
       </c>
@@ -6730,21 +6714,21 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>334</v>
       </c>
@@ -6776,7 +6760,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="30">
         <v>1</v>
       </c>
@@ -6804,7 +6788,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="34"/>
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
@@ -6815,7 +6799,7 @@
       <c r="H3" s="34"/>
       <c r="I3" s="34"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -6852,44 +6836,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="3.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.6640625" customWidth="1"/>
-    <col min="8" max="8" width="3.6640625" customWidth="1"/>
-    <col min="10" max="10" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.7109375" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="10" max="10" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.15">
-      <c r="A3" s="59" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="59"/>
+      <c r="G3" s="55"/>
       <c r="I3" t="s">
         <v>11</v>
       </c>
@@ -6897,28 +6881,28 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.15">
-      <c r="A4" s="60" t="s">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="60"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="G4" s="56"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
       <c r="E5" s="5">
         <f>VLOOKUP(B5,References!A2:B8,2,FALSE)</f>
         <v>3</v>
@@ -6934,15 +6918,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="5">
         <f>VLOOKUP(B6,References!C2:D6,2,FALSE)</f>
         <v>4</v>
@@ -6958,15 +6942,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
       <c r="E7" s="5">
         <f>VLOOKUP(B7,References!E2:F6,2,FALSE)</f>
         <v>0</v>
@@ -6982,17 +6966,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
       <c r="E8" s="5">
-        <f>VLOOKUP(B8,[1]Sheet3!G2:H8,2,FALSE)</f>
+        <f>VLOOKUP(B8,References!G3:H8,2,FALSE)</f>
         <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -7006,7 +6990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -7016,29 +7000,29 @@
       <c r="G9" s="8"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.15">
-      <c r="A10" s="60" t="s">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="60"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="5">
         <f>VLOOKUP(B11,References!I2:J7,2,FALSE)</f>
         <v>1</v>
@@ -7054,15 +7038,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
       <c r="E12" s="5">
         <f>VLOOKUP(B12,References!K$2:L$7,2,FALSE)</f>
         <v>5</v>
@@ -7078,15 +7062,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="5">
         <f>VLOOKUP(B13,References!M$2:N$7,2,FALSE)</f>
         <v>4</v>
@@ -7102,15 +7086,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
       <c r="E14" s="5">
         <f>VLOOKUP(B14,References!O$2:P$7,2,FALSE)</f>
         <v>3</v>
@@ -7126,57 +7110,57 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="61" t="s">
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="57">
+      <c r="B16" s="53">
         <f>IFERROR(AVERAGE(E5:E8,E11:E14),"All factors require a selection.")</f>
         <v>2.75</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="62" t="s">
+      <c r="F16" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="57">
+      <c r="G16" s="53">
         <f>IFERROR(AVERAGE(H5:H8,H11:H14),"All factors require a selection.")</f>
         <v>2.625</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="61"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="57"/>
-    </row>
-    <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B20" s="51" t="s">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="57"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="53"/>
+    </row>
+    <row r="20" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B20" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52" t="str">
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="62" t="str">
         <f>IFERROR(IF(AND($B$16&lt;3,$G$16&lt;3),"Note",IF(OR(AND($B$16&lt;3,$G$16&gt;=3,$G$16&lt;6),AND($B$16&gt;=3,$B$16&lt;6,$G$16&lt;3)),"Low",IF(OR(AND($B16&lt;3,$G16&gt;=6),AND($B16&gt;=3,$B16&lt;6,$G16&gt;=3,$G16&lt;6),AND($B16&gt;=6,$G16&lt;3)),"MODERATE",IF(OR(AND($B16&gt;=6,$B16&gt;=3,$G16&lt;6),AND($B16&gt;=3,$B16&lt;6,$G16&gt;6)),"High","Critical")))),"Note")</f>
         <v>Note</v>
       </c>
-      <c r="F20" s="52"/>
+      <c r="F20" s="62"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="53" t="s">
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>52</v>
       </c>
@@ -7194,7 +7178,7 @@
       </c>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="str">
         <f>IF($B16&lt;3,"-&gt;Low&lt;-","Low")</f>
         <v>-&gt;Low&lt;-</v>
@@ -7213,7 +7197,7 @@
       </c>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="str">
         <f>IF(AND($B16&gt;=3,$B16&lt;6),"-&gt;Moderate&lt;-","Moderate")</f>
         <v>Moderate</v>
@@ -7232,7 +7216,7 @@
       </c>
       <c r="F25" s="15"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="str">
         <f>IF($B16&gt;=6,"-&gt;High&lt;-","High")</f>
         <v>High</v>
@@ -7253,6 +7237,12 @@
   </sheetData>
   <dataConsolidate function="varp"/>
   <mergeCells count="22">
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="G16:G17"/>
@@ -7269,12 +7259,6 @@
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="E20:F20">
@@ -7385,31 +7369,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>15</v>
       </c>
@@ -7443,7 +7427,7 @@
       </c>
       <c r="P1" s="7"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>53</v>
       </c>
@@ -7493,7 +7477,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>55</v>
       </c>
@@ -7543,7 +7527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>57</v>
       </c>
@@ -7593,7 +7577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>61</v>
       </c>
@@ -7643,7 +7627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
@@ -7693,7 +7677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>73</v>
       </c>
@@ -7735,7 +7719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>78</v>
       </c>
@@ -7761,7 +7745,7 @@
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
     </row>
-    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>17</v>
       </c>
@@ -7795,7 +7779,7 @@
       </c>
       <c r="P10" s="9"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>53</v>
       </c>
@@ -7845,7 +7829,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
@@ -7895,7 +7879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>80</v>
       </c>
@@ -7945,7 +7929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
@@ -7995,7 +7979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>94</v>
       </c>
@@ -8045,7 +8029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>99</v>
       </c>
@@ -8087,7 +8071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">

</xml_diff>

<commit_message>
a few tools are added to the tools column based on the OWASP Testing guide v.4: DotDotPwn to OTG-AUTHZ-001, Webscarab to Authorization Tests, Errormint to OTG-ERROR tests, DOMinator to OTG-CLIENT-004 and OTG-CLIENT-006
</commit_message>
<xml_diff>
--- a/OWASPv4_Checklist.xlsx
+++ b/OWASPv4_Checklist.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\OWASP-Testing-Checklist\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="465" windowWidth="22740" windowHeight="12735" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Testing Checklist" sheetId="1" r:id="rId1"/>
@@ -36,7 +31,7 @@
     <definedName name="result">'Testing Checklist'!$A$128:$A$130</definedName>
     <definedName name="SkillRequired">References!$A$3:$A$8</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -52,7 +47,7 @@
     <author>pphongthiproek</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0" shapeId="0">
+    <comment ref="A5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="1" shapeId="0">
+    <comment ref="F5" authorId="1">
       <text>
         <r>
           <rPr>
@@ -80,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="1" shapeId="0">
+    <comment ref="F6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -108,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="1" shapeId="0">
+    <comment ref="A7" authorId="1">
       <text>
         <r>
           <rPr>
@@ -122,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="1" shapeId="0">
+    <comment ref="F7" authorId="1">
       <text>
         <r>
           <rPr>
@@ -136,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="1" shapeId="0">
+    <comment ref="A8" authorId="1">
       <text>
         <r>
           <rPr>
@@ -150,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="1" shapeId="0">
+    <comment ref="F8" authorId="1">
       <text>
         <r>
           <rPr>
@@ -164,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="1" shapeId="0">
+    <comment ref="A11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -178,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="1" shapeId="0">
+    <comment ref="F11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -192,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="1" shapeId="0">
+    <comment ref="A12" authorId="1">
       <text>
         <r>
           <rPr>
@@ -206,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="1" shapeId="0">
+    <comment ref="F12" authorId="1">
       <text>
         <r>
           <rPr>
@@ -220,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="1" shapeId="0">
+    <comment ref="A13" authorId="1">
       <text>
         <r>
           <rPr>
@@ -234,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="1" shapeId="0">
+    <comment ref="F13" authorId="1">
       <text>
         <r>
           <rPr>
@@ -248,7 +243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="1" shapeId="0">
+    <comment ref="A14" authorId="1">
       <text>
         <r>
           <rPr>
@@ -262,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="1" shapeId="0">
+    <comment ref="F14" authorId="1">
       <text>
         <r>
           <rPr>
@@ -281,7 +276,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="469">
   <si>
     <t>Information Gathering</t>
   </si>
@@ -1743,6 +1738,18 @@
   </si>
   <si>
     <t>Burp Proxy, ZAP, Liffy, Panoptic</t>
+  </si>
+  <si>
+    <t>Burp Proxy, ZAP, Wfuzz,DotDotPwn</t>
+  </si>
+  <si>
+    <t>Burp Proxy (Autorize), ZAP, WebScarab</t>
+  </si>
+  <si>
+    <t>Burp Proxy, ZAP, Errormint</t>
+  </si>
+  <si>
+    <t>Burp Proxy, ZAP, DOMinator</t>
   </si>
 </sst>
 </file>
@@ -2164,6 +2171,18 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2189,23 +2208,47 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="126">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2532,24 +2575,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="9"/>
         <color theme="0" tint="-0.499984740745262"/>
         <name val="Arial"/>
@@ -2880,24 +2905,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3644,14 +3651,14 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table61415" displayName="Table61415" ref="A96:F99" totalsRowShown="0" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table61415" displayName="Table61415" ref="A96:F99" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A96:F99"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Cryptography" dataDxfId="26"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="25"/>
-    <tableColumn id="3" name="Description" dataDxfId="24"/>
-    <tableColumn id="4" name="Tools" dataDxfId="23"/>
-    <tableColumn id="5" name="Result" dataDxfId="22"/>
+    <tableColumn id="1" name="Cryptography" dataDxfId="28"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="27"/>
+    <tableColumn id="3" name="Description" dataDxfId="26"/>
+    <tableColumn id="4" name="Tools" dataDxfId="25"/>
+    <tableColumn id="5" name="Result" dataDxfId="24"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3659,14 +3666,14 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table616" displayName="Table616" ref="A112:F124" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table616" displayName="Table616" ref="A112:F124" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A112:F124"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Client Side Testing" dataDxfId="20"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="19"/>
-    <tableColumn id="3" name="Description" dataDxfId="18"/>
-    <tableColumn id="4" name="Tools" dataDxfId="17"/>
-    <tableColumn id="5" name="Result" dataDxfId="16"/>
+    <tableColumn id="1" name="Client Side Testing" dataDxfId="22"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="21"/>
+    <tableColumn id="3" name="Description" dataDxfId="20"/>
+    <tableColumn id="4" name="Tools" dataDxfId="19"/>
+    <tableColumn id="5" name="Result" dataDxfId="18"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3725,8 +3732,8 @@
     <tableColumn id="1" name="Authorization Testing " dataDxfId="56"/>
     <tableColumn id="2" name="Test Name" dataDxfId="55"/>
     <tableColumn id="3" name="Description" dataDxfId="54"/>
-    <tableColumn id="4" name="Tools" dataDxfId="53"/>
-    <tableColumn id="5" name="Result" dataDxfId="52"/>
+    <tableColumn id="4" name="Tools" dataDxfId="1"/>
+    <tableColumn id="5" name="Result" dataDxfId="53"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3734,14 +3741,14 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A101:F110" totalsRowShown="0" headerRowDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A101:F110" totalsRowShown="0" headerRowDxfId="52">
   <autoFilter ref="A101:F110"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Business logic Testing" dataDxfId="50"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="49"/>
-    <tableColumn id="3" name="Description" dataDxfId="48"/>
-    <tableColumn id="4" name="Tools" dataDxfId="47"/>
-    <tableColumn id="5" name="Result" dataDxfId="46"/>
+    <tableColumn id="1" name="Business logic Testing" dataDxfId="51"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="50"/>
+    <tableColumn id="3" name="Description" dataDxfId="49"/>
+    <tableColumn id="4" name="Tools" dataDxfId="48"/>
+    <tableColumn id="5" name="Result" dataDxfId="47"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3749,14 +3756,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A63:F90" totalsRowShown="0" headerRowDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A63:F90" totalsRowShown="0" headerRowDxfId="46">
   <autoFilter ref="A63:F90"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Data Validation Testing" dataDxfId="44"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="43"/>
-    <tableColumn id="3" name="Description" dataDxfId="42"/>
-    <tableColumn id="4" name="Tools" dataDxfId="41"/>
-    <tableColumn id="5" name="Result" dataDxfId="40"/>
+    <tableColumn id="1" name="Data Validation Testing" dataDxfId="45"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="44"/>
+    <tableColumn id="3" name="Description" dataDxfId="43"/>
+    <tableColumn id="4" name="Tools" dataDxfId="42"/>
+    <tableColumn id="5" name="Result" dataDxfId="41"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3764,14 +3771,14 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table29" displayName="Table29" ref="A26:F33" totalsRowShown="0" headerRowDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table29" displayName="Table29" ref="A26:F33" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A26:F33"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Identity Management Testing" dataDxfId="38"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="37"/>
-    <tableColumn id="3" name="Description" dataDxfId="36"/>
-    <tableColumn id="4" name="Tools" dataDxfId="35"/>
-    <tableColumn id="5" name="Result" dataDxfId="34"/>
+    <tableColumn id="1" name="Identity Management Testing" dataDxfId="39"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="38"/>
+    <tableColumn id="3" name="Description" dataDxfId="37"/>
+    <tableColumn id="4" name="Tools" dataDxfId="36"/>
+    <tableColumn id="5" name="Result" dataDxfId="35"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3779,14 +3786,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table614" displayName="Table614" ref="A92:F94" totalsRowShown="0" headerRowDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table614" displayName="Table614" ref="A92:F94" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="A92:F94"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Error Handling" dataDxfId="32"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="31"/>
-    <tableColumn id="3" name="Description" dataDxfId="30"/>
-    <tableColumn id="4" name="Tools" dataDxfId="29"/>
-    <tableColumn id="5" name="Result" dataDxfId="28"/>
+    <tableColumn id="1" name="Error Handling" dataDxfId="33"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="32"/>
+    <tableColumn id="3" name="Description" dataDxfId="31"/>
+    <tableColumn id="4" name="Tools" dataDxfId="0"/>
+    <tableColumn id="5" name="Result" dataDxfId="30"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3794,9 +3801,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Ofis Teması">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Ofis">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3834,9 +3841,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Ofis">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3871,7 +3878,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3906,7 +3913,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Ofis">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4082,8 +4089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4848,7 +4855,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="20" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" s="20" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
         <v>196</v>
       </c>
@@ -4859,13 +4866,13 @@
         <v>369</v>
       </c>
       <c r="D48" s="44" t="s">
-        <v>446</v>
+        <v>465</v>
       </c>
       <c r="E48" s="24" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
         <v>197</v>
       </c>
@@ -4876,13 +4883,13 @@
         <v>370</v>
       </c>
       <c r="D49" s="44" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="E49" s="24" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
         <v>198</v>
       </c>
@@ -4893,7 +4900,7 @@
         <v>109</v>
       </c>
       <c r="D50" s="44" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="E50" s="24" t="s">
         <v>123</v>
@@ -5584,7 +5591,7 @@
         <v>411</v>
       </c>
       <c r="D93" s="44" t="s">
-        <v>442</v>
+        <v>467</v>
       </c>
       <c r="E93" s="24" t="s">
         <v>123</v>
@@ -5602,7 +5609,7 @@
         <v>412</v>
       </c>
       <c r="D94" s="44" t="s">
-        <v>442</v>
+        <v>467</v>
       </c>
       <c r="E94" s="24" t="s">
         <v>123</v>
@@ -5969,7 +5976,7 @@
         <v>429</v>
       </c>
       <c r="D116" s="44" t="s">
-        <v>442</v>
+        <v>468</v>
       </c>
       <c r="E116" s="38" t="s">
         <v>123</v>
@@ -6005,7 +6012,7 @@
         <v>432</v>
       </c>
       <c r="D118" s="44" t="s">
-        <v>442</v>
+        <v>468</v>
       </c>
       <c r="E118" s="38" t="s">
         <v>123</v>
@@ -6812,19 +6819,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>"Note"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
       <formula>"Moderate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6836,7 +6843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -6852,28 +6859,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="55" t="s">
+      <c r="F3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="55"/>
+      <c r="G3" s="59"/>
       <c r="I3" t="s">
         <v>11</v>
       </c>
@@ -6882,27 +6889,27 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="56"/>
+      <c r="G4" s="60"/>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="5">
         <f>VLOOKUP(B5,References!A2:B8,2,FALSE)</f>
         <v>3</v>
@@ -6922,11 +6929,11 @@
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
       <c r="E6" s="5">
         <f>VLOOKUP(B6,References!C2:D6,2,FALSE)</f>
         <v>4</v>
@@ -6946,11 +6953,11 @@
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
       <c r="E7" s="5">
         <f>VLOOKUP(B7,References!E2:F6,2,FALSE)</f>
         <v>0</v>
@@ -6970,11 +6977,11 @@
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
       <c r="E8" s="5">
         <f>VLOOKUP(B8,References!G3:H8,2,FALSE)</f>
         <v>2</v>
@@ -7001,28 +7008,28 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="56"/>
+      <c r="G10" s="60"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
       <c r="E11" s="5">
         <f>VLOOKUP(B11,References!I2:J7,2,FALSE)</f>
         <v>1</v>
@@ -7042,11 +7049,11 @@
       <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
       <c r="E12" s="5">
         <f>VLOOKUP(B12,References!K$2:L$7,2,FALSE)</f>
         <v>5</v>
@@ -7066,11 +7073,11 @@
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
       <c r="E13" s="5">
         <f>VLOOKUP(B13,References!M$2:N$7,2,FALSE)</f>
         <v>4</v>
@@ -7090,11 +7097,11 @@
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
       <c r="E14" s="5">
         <f>VLOOKUP(B14,References!O$2:P$7,2,FALSE)</f>
         <v>3</v>
@@ -7114,51 +7121,51 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="53">
+      <c r="B16" s="57">
         <f>IFERROR(AVERAGE(E5:E8,E11:E14),"All factors require a selection.")</f>
         <v>2.75</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="58" t="s">
+      <c r="F16" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="53">
+      <c r="G16" s="57">
         <f>IFERROR(AVERAGE(H5:H8,H11:H14),"All factors require a selection.")</f>
         <v>2.625</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="57"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="53"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="57"/>
     </row>
     <row r="20" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="62" t="str">
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="52" t="str">
         <f>IFERROR(IF(AND($B$16&lt;3,$G$16&lt;3),"Note",IF(OR(AND($B$16&lt;3,$G$16&gt;=3,$G$16&lt;6),AND($B$16&gt;=3,$B$16&lt;6,$G$16&lt;3)),"Low",IF(OR(AND($B16&lt;3,$G16&gt;=6),AND($B16&gt;=3,$B16&lt;6,$G16&gt;=3,$G16&lt;6),AND($B16&gt;=6,$G16&lt;3)),"MODERATE",IF(OR(AND($B16&gt;=6,$B16&gt;=3,$G16&lt;6),AND($B16&gt;=3,$B16&lt;6,$G16&gt;6)),"High","Critical")))),"Note")</f>
         <v>Note</v>
       </c>
-      <c r="F20" s="62"/>
+      <c r="F20" s="52"/>
       <c r="G20" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -7237,12 +7244,6 @@
   </sheetData>
   <dataConsolidate function="varp"/>
   <mergeCells count="22">
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="G16:G17"/>
@@ -7259,52 +7260,58 @@
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="E20:F20">
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="critical">
+    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="critical">
       <formula>NOT(ISERROR(SEARCH("critical",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="high">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="high">
       <formula>NOT(ISERROR(SEARCH("high",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="moderate">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="moderate">
       <formula>NOT(ISERROR(SEARCH("moderate",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="low">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="low">
       <formula>NOT(ISERROR(SEARCH("low",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="Note">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="Note">
       <formula>NOT(ISERROR(SEARCH("Note",E20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:A26 B23:D23">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",A23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:D26 A24:A26">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",A23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",D25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",C25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",B26)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
typo correction on the previous commit
</commit_message>
<xml_diff>
--- a/OWASPv4_Checklist.xlsx
+++ b/OWASPv4_Checklist.xlsx
@@ -1740,9 +1740,6 @@
     <t>Burp Proxy, ZAP, Liffy, Panoptic</t>
   </si>
   <si>
-    <t>Burp Proxy, ZAP, Wfuzz,DotDotPwn</t>
-  </si>
-  <si>
     <t>Burp Proxy (Autorize), ZAP, WebScarab</t>
   </si>
   <si>
@@ -1750,6 +1747,9 @@
   </si>
   <si>
     <t>Burp Proxy, ZAP, DOMinator</t>
+  </si>
+  <si>
+    <t>Burp Proxy, ZAP, Wfuzz, DotDotPwn</t>
   </si>
 </sst>
 </file>
@@ -2171,18 +2171,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2208,47 +2196,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="126">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2575,6 +2539,24 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="9"/>
         <color theme="0" tint="-0.499984740745262"/>
         <name val="Arial"/>
@@ -2905,6 +2887,24 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3651,14 +3651,14 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table61415" displayName="Table61415" ref="A96:F99" totalsRowShown="0" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table61415" displayName="Table61415" ref="A96:F99" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="A96:F99"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Cryptography" dataDxfId="28"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="27"/>
-    <tableColumn id="3" name="Description" dataDxfId="26"/>
-    <tableColumn id="4" name="Tools" dataDxfId="25"/>
-    <tableColumn id="5" name="Result" dataDxfId="24"/>
+    <tableColumn id="1" name="Cryptography" dataDxfId="26"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="25"/>
+    <tableColumn id="3" name="Description" dataDxfId="24"/>
+    <tableColumn id="4" name="Tools" dataDxfId="23"/>
+    <tableColumn id="5" name="Result" dataDxfId="22"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3666,14 +3666,14 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table616" displayName="Table616" ref="A112:F124" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table616" displayName="Table616" ref="A112:F124" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="A112:F124"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Client Side Testing" dataDxfId="22"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="21"/>
-    <tableColumn id="3" name="Description" dataDxfId="20"/>
-    <tableColumn id="4" name="Tools" dataDxfId="19"/>
-    <tableColumn id="5" name="Result" dataDxfId="18"/>
+    <tableColumn id="1" name="Client Side Testing" dataDxfId="20"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="19"/>
+    <tableColumn id="3" name="Description" dataDxfId="18"/>
+    <tableColumn id="4" name="Tools" dataDxfId="17"/>
+    <tableColumn id="5" name="Result" dataDxfId="16"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3732,8 +3732,8 @@
     <tableColumn id="1" name="Authorization Testing " dataDxfId="56"/>
     <tableColumn id="2" name="Test Name" dataDxfId="55"/>
     <tableColumn id="3" name="Description" dataDxfId="54"/>
-    <tableColumn id="4" name="Tools" dataDxfId="1"/>
-    <tableColumn id="5" name="Result" dataDxfId="53"/>
+    <tableColumn id="4" name="Tools" dataDxfId="53"/>
+    <tableColumn id="5" name="Result" dataDxfId="52"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3741,14 +3741,14 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A101:F110" totalsRowShown="0" headerRowDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A101:F110" totalsRowShown="0" headerRowDxfId="51">
   <autoFilter ref="A101:F110"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Business logic Testing" dataDxfId="51"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="50"/>
-    <tableColumn id="3" name="Description" dataDxfId="49"/>
-    <tableColumn id="4" name="Tools" dataDxfId="48"/>
-    <tableColumn id="5" name="Result" dataDxfId="47"/>
+    <tableColumn id="1" name="Business logic Testing" dataDxfId="50"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="49"/>
+    <tableColumn id="3" name="Description" dataDxfId="48"/>
+    <tableColumn id="4" name="Tools" dataDxfId="47"/>
+    <tableColumn id="5" name="Result" dataDxfId="46"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3756,14 +3756,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A63:F90" totalsRowShown="0" headerRowDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A63:F90" totalsRowShown="0" headerRowDxfId="45">
   <autoFilter ref="A63:F90"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Data Validation Testing" dataDxfId="45"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="44"/>
-    <tableColumn id="3" name="Description" dataDxfId="43"/>
-    <tableColumn id="4" name="Tools" dataDxfId="42"/>
-    <tableColumn id="5" name="Result" dataDxfId="41"/>
+    <tableColumn id="1" name="Data Validation Testing" dataDxfId="44"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="43"/>
+    <tableColumn id="3" name="Description" dataDxfId="42"/>
+    <tableColumn id="4" name="Tools" dataDxfId="41"/>
+    <tableColumn id="5" name="Result" dataDxfId="40"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3771,14 +3771,14 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table29" displayName="Table29" ref="A26:F33" totalsRowShown="0" headerRowDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table29" displayName="Table29" ref="A26:F33" totalsRowShown="0" headerRowDxfId="39">
   <autoFilter ref="A26:F33"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Identity Management Testing" dataDxfId="39"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="38"/>
-    <tableColumn id="3" name="Description" dataDxfId="37"/>
-    <tableColumn id="4" name="Tools" dataDxfId="36"/>
-    <tableColumn id="5" name="Result" dataDxfId="35"/>
+    <tableColumn id="1" name="Identity Management Testing" dataDxfId="38"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="37"/>
+    <tableColumn id="3" name="Description" dataDxfId="36"/>
+    <tableColumn id="4" name="Tools" dataDxfId="35"/>
+    <tableColumn id="5" name="Result" dataDxfId="34"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3786,14 +3786,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table614" displayName="Table614" ref="A92:F94" totalsRowShown="0" headerRowDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table614" displayName="Table614" ref="A92:F94" totalsRowShown="0" headerRowDxfId="33">
   <autoFilter ref="A92:F94"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Error Handling" dataDxfId="33"/>
-    <tableColumn id="2" name="Test Name" dataDxfId="32"/>
-    <tableColumn id="3" name="Description" dataDxfId="31"/>
-    <tableColumn id="4" name="Tools" dataDxfId="0"/>
-    <tableColumn id="5" name="Result" dataDxfId="30"/>
+    <tableColumn id="1" name="Error Handling" dataDxfId="32"/>
+    <tableColumn id="2" name="Test Name" dataDxfId="31"/>
+    <tableColumn id="3" name="Description" dataDxfId="30"/>
+    <tableColumn id="4" name="Tools" dataDxfId="29"/>
+    <tableColumn id="5" name="Result" dataDxfId="28"/>
     <tableColumn id="6" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4089,8 +4089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4866,7 +4866,7 @@
         <v>369</v>
       </c>
       <c r="D48" s="44" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="E48" s="24" t="s">
         <v>123</v>
@@ -4883,7 +4883,7 @@
         <v>370</v>
       </c>
       <c r="D49" s="44" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E49" s="24" t="s">
         <v>123</v>
@@ -4900,7 +4900,7 @@
         <v>109</v>
       </c>
       <c r="D50" s="44" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E50" s="24" t="s">
         <v>123</v>
@@ -5591,7 +5591,7 @@
         <v>411</v>
       </c>
       <c r="D93" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E93" s="24" t="s">
         <v>123</v>
@@ -5609,7 +5609,7 @@
         <v>412</v>
       </c>
       <c r="D94" s="44" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E94" s="24" t="s">
         <v>123</v>
@@ -5976,7 +5976,7 @@
         <v>429</v>
       </c>
       <c r="D116" s="44" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E116" s="38" t="s">
         <v>123</v>
@@ -6012,7 +6012,7 @@
         <v>432</v>
       </c>
       <c r="D118" s="44" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E118" s="38" t="s">
         <v>123</v>
@@ -6819,19 +6819,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"Note"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"Moderate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6859,28 +6859,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="59"/>
+      <c r="G3" s="55"/>
       <c r="I3" t="s">
         <v>11</v>
       </c>
@@ -6889,27 +6889,27 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="60"/>
+      <c r="G4" s="56"/>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
       <c r="E5" s="5">
         <f>VLOOKUP(B5,References!A2:B8,2,FALSE)</f>
         <v>3</v>
@@ -6929,11 +6929,11 @@
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="5">
         <f>VLOOKUP(B6,References!C2:D6,2,FALSE)</f>
         <v>4</v>
@@ -6953,11 +6953,11 @@
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
       <c r="E7" s="5">
         <f>VLOOKUP(B7,References!E2:F6,2,FALSE)</f>
         <v>0</v>
@@ -6977,11 +6977,11 @@
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
       <c r="E8" s="5">
         <f>VLOOKUP(B8,References!G3:H8,2,FALSE)</f>
         <v>2</v>
@@ -7008,28 +7008,28 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="60"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="5">
         <f>VLOOKUP(B11,References!I2:J7,2,FALSE)</f>
         <v>1</v>
@@ -7049,11 +7049,11 @@
       <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
       <c r="E12" s="5">
         <f>VLOOKUP(B12,References!K$2:L$7,2,FALSE)</f>
         <v>5</v>
@@ -7073,11 +7073,11 @@
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="5">
         <f>VLOOKUP(B13,References!M$2:N$7,2,FALSE)</f>
         <v>4</v>
@@ -7097,11 +7097,11 @@
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
       <c r="E14" s="5">
         <f>VLOOKUP(B14,References!O$2:P$7,2,FALSE)</f>
         <v>3</v>
@@ -7121,51 +7121,51 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="57">
+      <c r="B16" s="53">
         <f>IFERROR(AVERAGE(E5:E8,E11:E14),"All factors require a selection.")</f>
         <v>2.75</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="62" t="s">
+      <c r="F16" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="57">
+      <c r="G16" s="53">
         <f>IFERROR(AVERAGE(H5:H8,H11:H14),"All factors require a selection.")</f>
         <v>2.625</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="61"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="57"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="53"/>
     </row>
     <row r="20" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52" t="str">
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="62" t="str">
         <f>IFERROR(IF(AND($B$16&lt;3,$G$16&lt;3),"Note",IF(OR(AND($B$16&lt;3,$G$16&gt;=3,$G$16&lt;6),AND($B$16&gt;=3,$B$16&lt;6,$G$16&lt;3)),"Low",IF(OR(AND($B16&lt;3,$G16&gt;=6),AND($B16&gt;=3,$B16&lt;6,$G16&gt;=3,$G16&lt;6),AND($B16&gt;=6,$G16&lt;3)),"MODERATE",IF(OR(AND($B16&gt;=6,$B16&gt;=3,$G16&lt;6),AND($B16&gt;=3,$B16&lt;6,$G16&gt;6)),"High","Critical")))),"Note")</f>
         <v>Note</v>
       </c>
-      <c r="F20" s="52"/>
+      <c r="F20" s="62"/>
       <c r="G20" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -7244,6 +7244,12 @@
   </sheetData>
   <dataConsolidate function="varp"/>
   <mergeCells count="22">
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B16:D17"/>
     <mergeCell ref="G16:G17"/>
@@ -7260,58 +7266,52 @@
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="E20:F20">
-    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="critical">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="critical">
       <formula>NOT(ISERROR(SEARCH("critical",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="high">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="high">
       <formula>NOT(ISERROR(SEARCH("high",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="moderate">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="moderate">
       <formula>NOT(ISERROR(SEARCH("moderate",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="low">
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="low">
       <formula>NOT(ISERROR(SEARCH("low",E20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="Note">
+    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="Note">
       <formula>NOT(ISERROR(SEARCH("Note",E20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:A26 B23:D23">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",A23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:D26 A24:A26">
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",A23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",D25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",C25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH("&lt;",B26)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>